<commit_message>
Returns results in Learners + Fix policy gradient + Fix transition model
</commit_message>
<xml_diff>
--- a/Importance sampling/Learning.xlsx
+++ b/Importance sampling/Learning.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7200" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7200" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -3503,6 +3504,484 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja3!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja3!$L$2:$L$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>14.318533491889999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.414414679110005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.44275148521</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.257884062650003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.695360480610002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.365558641290001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.532961476819999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.893088598570003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17.961647312030003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18.32683854723</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.389677520379998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.865121444000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18.225709010479996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18.847458747019999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20.785380650420002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>22.301376531820001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.944843787330001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22.93281357107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5084-40C1-90C2-C660617C9E2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja3!$I$22:$I$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>18.953815040385713</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.92738263737143</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.759941494600003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.180318400228568</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.467442342785713</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.583594417871428</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.267883428899999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.47916786157143</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.991383433799999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.002284704200001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19.568578072871428</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.396320613471428</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.083285800942853</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20.474963635642858</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21.193973629442858</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21.522686796742857</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21.338103808571429</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22.537898294371434</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8BA4-466E-9B73-D94CEE3882DD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="413077968"/>
+        <c:axId val="413077640"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="413077968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="413077640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="413077640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="413077968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3544,6 +4023,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4615,6 +5134,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4664,6 +5699,41 @@
       <xdr:colOff>601732</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>34373</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4985,7 +6055,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5608,8 +6678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6726,4 +7796,1263 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:L39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>200</v>
+      </c>
+      <c r="B2">
+        <v>10.601486548900001</v>
+      </c>
+      <c r="C2">
+        <v>15.939604344399999</v>
+      </c>
+      <c r="D2">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="E2">
+        <v>10.5946171508</v>
+      </c>
+      <c r="F2">
+        <v>10.6731621952</v>
+      </c>
+      <c r="G2">
+        <v>17.742151272600001</v>
+      </c>
+      <c r="H2">
+        <v>10.672960850400001</v>
+      </c>
+      <c r="I2">
+        <v>10.5907853135</v>
+      </c>
+      <c r="J2">
+        <v>22.1640838575</v>
+      </c>
+      <c r="K2">
+        <v>10.5838429746</v>
+      </c>
+      <c r="L2">
+        <f>AVERAGE(B2:K2)</f>
+        <v>14.318533491889999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>400</v>
+      </c>
+      <c r="B3">
+        <v>23.1310054108</v>
+      </c>
+      <c r="C3">
+        <v>22.076886660300001</v>
+      </c>
+      <c r="D3">
+        <v>22.201592438700001</v>
+      </c>
+      <c r="E3">
+        <v>23.177106524300001</v>
+      </c>
+      <c r="F3">
+        <v>10.6181459219</v>
+      </c>
+      <c r="G3">
+        <v>10.579384724800001</v>
+      </c>
+      <c r="H3">
+        <v>10.5850956501</v>
+      </c>
+      <c r="I3">
+        <v>10.588632279700001</v>
+      </c>
+      <c r="J3">
+        <v>10.579384724800001</v>
+      </c>
+      <c r="K3">
+        <v>10.6069124557</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L19" si="0">AVERAGE(B3:K3)</f>
+        <v>15.414414679110005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>600</v>
+      </c>
+      <c r="B4">
+        <v>10.5999659486</v>
+      </c>
+      <c r="C4">
+        <v>20.364806113499998</v>
+      </c>
+      <c r="D4">
+        <v>17.3900776061</v>
+      </c>
+      <c r="E4">
+        <v>22.1640838575</v>
+      </c>
+      <c r="F4">
+        <v>23.2769340081</v>
+      </c>
+      <c r="G4">
+        <v>16.212288403100001</v>
+      </c>
+      <c r="H4">
+        <v>18.395586652999999</v>
+      </c>
+      <c r="I4">
+        <v>10.585434402700001</v>
+      </c>
+      <c r="J4">
+        <v>14.596793273699999</v>
+      </c>
+      <c r="K4">
+        <v>20.841544585800001</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>17.44275148521</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>800</v>
+      </c>
+      <c r="B5">
+        <v>22.763575522899998</v>
+      </c>
+      <c r="C5">
+        <v>13.8318642896</v>
+      </c>
+      <c r="D5">
+        <v>15.634819853</v>
+      </c>
+      <c r="E5">
+        <v>22.494409750999999</v>
+      </c>
+      <c r="F5">
+        <v>11.141266587900001</v>
+      </c>
+      <c r="G5">
+        <v>17.838305868599999</v>
+      </c>
+      <c r="H5">
+        <v>22.365442422200001</v>
+      </c>
+      <c r="I5">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="J5">
+        <v>11.3861744854</v>
+      </c>
+      <c r="K5">
+        <v>11.500341434899999</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>17.257884062650003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1000</v>
+      </c>
+      <c r="B6">
+        <v>13.8306692495</v>
+      </c>
+      <c r="C6">
+        <v>10.6071556824</v>
+      </c>
+      <c r="D6">
+        <v>20.491630696200001</v>
+      </c>
+      <c r="E6">
+        <v>23.270994977200001</v>
+      </c>
+      <c r="F6">
+        <v>23.4052460419</v>
+      </c>
+      <c r="G6">
+        <v>21.777188501400001</v>
+      </c>
+      <c r="H6">
+        <v>18.171914464699999</v>
+      </c>
+      <c r="I6">
+        <v>21.211135779999999</v>
+      </c>
+      <c r="J6">
+        <v>15.273020135199999</v>
+      </c>
+      <c r="K6">
+        <v>18.914649277599999</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>18.695360480610002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2000</v>
+      </c>
+      <c r="B7">
+        <v>10.610604756200001</v>
+      </c>
+      <c r="C7">
+        <v>22.861574891</v>
+      </c>
+      <c r="D7">
+        <v>10.6009931684</v>
+      </c>
+      <c r="E7">
+        <v>23.622600292000001</v>
+      </c>
+      <c r="F7">
+        <v>23.546704580699998</v>
+      </c>
+      <c r="G7">
+        <v>10.6564396415</v>
+      </c>
+      <c r="H7">
+        <v>23.423783103600002</v>
+      </c>
+      <c r="I7">
+        <v>22.5856389789</v>
+      </c>
+      <c r="J7">
+        <v>23.044393530499999</v>
+      </c>
+      <c r="K7">
+        <v>22.702853470099999</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>19.365558641290001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3000</v>
+      </c>
+      <c r="B8">
+        <v>22.536132958700001</v>
+      </c>
+      <c r="C8">
+        <v>20.6794648238</v>
+      </c>
+      <c r="D8">
+        <v>16.2748738433</v>
+      </c>
+      <c r="E8">
+        <v>17.494483630600001</v>
+      </c>
+      <c r="F8">
+        <v>19.403243316200001</v>
+      </c>
+      <c r="G8">
+        <v>23.296600351199999</v>
+      </c>
+      <c r="H8">
+        <v>20.5097114201</v>
+      </c>
+      <c r="I8">
+        <v>18.971949753600001</v>
+      </c>
+      <c r="J8">
+        <v>23.272093933600001</v>
+      </c>
+      <c r="K8">
+        <v>22.891060737099998</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>20.532961476819999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4000</v>
+      </c>
+      <c r="B9">
+        <v>13.027275385999999</v>
+      </c>
+      <c r="C9">
+        <v>23.1757966634</v>
+      </c>
+      <c r="D9">
+        <v>14.877173190700001</v>
+      </c>
+      <c r="E9">
+        <v>22.643521164799999</v>
+      </c>
+      <c r="F9">
+        <v>19.695537118000001</v>
+      </c>
+      <c r="G9">
+        <v>22.826016247199998</v>
+      </c>
+      <c r="H9">
+        <v>20.255127214600002</v>
+      </c>
+      <c r="I9">
+        <v>14.089837681900001</v>
+      </c>
+      <c r="J9">
+        <v>23.233331421900001</v>
+      </c>
+      <c r="K9">
+        <v>15.1072698972</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>18.893088598570003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5000</v>
+      </c>
+      <c r="B10">
+        <v>13.275074177900001</v>
+      </c>
+      <c r="C10">
+        <v>12.5879267158</v>
+      </c>
+      <c r="D10">
+        <v>22.3162302428</v>
+      </c>
+      <c r="E10">
+        <v>22.604591012499998</v>
+      </c>
+      <c r="F10">
+        <v>21.829225460899998</v>
+      </c>
+      <c r="G10">
+        <v>12.573089277999999</v>
+      </c>
+      <c r="H10">
+        <v>22.769976071599999</v>
+      </c>
+      <c r="I10">
+        <v>13.893376571999999</v>
+      </c>
+      <c r="J10">
+        <v>15.059014522</v>
+      </c>
+      <c r="K10">
+        <v>22.7079690668</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>17.961647312030003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6000</v>
+      </c>
+      <c r="B11">
+        <v>17.382263971</v>
+      </c>
+      <c r="C11">
+        <v>19.134469431900001</v>
+      </c>
+      <c r="D11">
+        <v>20.418931603899999</v>
+      </c>
+      <c r="E11">
+        <v>22.608012347599999</v>
+      </c>
+      <c r="F11">
+        <v>20.967899976799998</v>
+      </c>
+      <c r="G11">
+        <v>12.680353694900001</v>
+      </c>
+      <c r="H11">
+        <v>18.91433507</v>
+      </c>
+      <c r="I11">
+        <v>14.3275574015</v>
+      </c>
+      <c r="J11">
+        <v>13.997646984199999</v>
+      </c>
+      <c r="K11">
+        <v>22.836914990499999</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>18.32683854723</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7000</v>
+      </c>
+      <c r="B12">
+        <v>14.894863062300001</v>
+      </c>
+      <c r="C12">
+        <v>22.8456212165</v>
+      </c>
+      <c r="D12">
+        <v>16.297448450299999</v>
+      </c>
+      <c r="E12">
+        <v>22.628258714099999</v>
+      </c>
+      <c r="F12">
+        <v>23.594011153899999</v>
+      </c>
+      <c r="G12">
+        <v>23.576879303199998</v>
+      </c>
+      <c r="H12">
+        <v>17.7378062907</v>
+      </c>
+      <c r="I12">
+        <v>14.026675572</v>
+      </c>
+      <c r="J12">
+        <v>13.7062207295</v>
+      </c>
+      <c r="K12">
+        <v>14.588990711299999</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>18.389677520379998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8000</v>
+      </c>
+      <c r="B13">
+        <v>16.146208116499999</v>
+      </c>
+      <c r="C13">
+        <v>19.300509550600001</v>
+      </c>
+      <c r="D13">
+        <v>15.7110425689</v>
+      </c>
+      <c r="E13">
+        <v>22.6258088702</v>
+      </c>
+      <c r="F13">
+        <v>22.9100988414</v>
+      </c>
+      <c r="G13">
+        <v>12.5117914632</v>
+      </c>
+      <c r="H13">
+        <v>20.127107546200001</v>
+      </c>
+      <c r="I13">
+        <v>14.018465856100001</v>
+      </c>
+      <c r="J13">
+        <v>13.3380751786</v>
+      </c>
+      <c r="K13">
+        <v>21.962106448299998</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>17.865121444000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9000</v>
+      </c>
+      <c r="B14">
+        <v>14.673169662799999</v>
+      </c>
+      <c r="C14">
+        <v>22.957701294700001</v>
+      </c>
+      <c r="D14">
+        <v>22.614969814599998</v>
+      </c>
+      <c r="E14">
+        <v>22.450290882400001</v>
+      </c>
+      <c r="F14">
+        <v>19.860966362500001</v>
+      </c>
+      <c r="G14">
+        <v>12.470912125</v>
+      </c>
+      <c r="H14">
+        <v>17.902257240299999</v>
+      </c>
+      <c r="I14">
+        <v>19.336035686799999</v>
+      </c>
+      <c r="J14">
+        <v>15.418752704299999</v>
+      </c>
+      <c r="K14">
+        <v>14.572034331399999</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>18.225709010479996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10000</v>
+      </c>
+      <c r="B15">
+        <v>18.058759019</v>
+      </c>
+      <c r="C15">
+        <v>22.939311194199998</v>
+      </c>
+      <c r="D15">
+        <v>20.410232609099999</v>
+      </c>
+      <c r="E15">
+        <v>22.637517446899999</v>
+      </c>
+      <c r="F15">
+        <v>22.981495905799999</v>
+      </c>
+      <c r="G15">
+        <v>12.5541145172</v>
+      </c>
+      <c r="H15">
+        <v>22.833874658100001</v>
+      </c>
+      <c r="I15">
+        <v>18.721046198700002</v>
+      </c>
+      <c r="J15">
+        <v>13.1109753891</v>
+      </c>
+      <c r="K15">
+        <v>14.227260532100001</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>18.847458747019999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>20000</v>
+      </c>
+      <c r="B16">
+        <v>22.5227268583</v>
+      </c>
+      <c r="C16">
+        <v>23.0087482506</v>
+      </c>
+      <c r="D16">
+        <v>22.717663445500001</v>
+      </c>
+      <c r="E16">
+        <v>22.640997028299999</v>
+      </c>
+      <c r="F16">
+        <v>23.578354868200002</v>
+      </c>
+      <c r="G16">
+        <v>12.7483748178</v>
+      </c>
+      <c r="H16">
+        <v>22.7450120791</v>
+      </c>
+      <c r="I16">
+        <v>20.5657818056</v>
+      </c>
+      <c r="J16">
+        <v>14.6566593762</v>
+      </c>
+      <c r="K16">
+        <v>22.669487974599999</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>20.785380650420002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>30000</v>
+      </c>
+      <c r="B17">
+        <v>22.5201111963</v>
+      </c>
+      <c r="C17">
+        <v>18.353464950100001</v>
+      </c>
+      <c r="D17">
+        <v>22.7251524297</v>
+      </c>
+      <c r="E17">
+        <v>22.639801839899999</v>
+      </c>
+      <c r="F17">
+        <v>23.5678746912</v>
+      </c>
+      <c r="G17">
+        <v>21.851854685799999</v>
+      </c>
+      <c r="H17">
+        <v>22.6955692053</v>
+      </c>
+      <c r="I17">
+        <v>22.487756491700001</v>
+      </c>
+      <c r="J17">
+        <v>23.499454893100001</v>
+      </c>
+      <c r="K17">
+        <v>22.6727249351</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>22.301376531820001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>40000</v>
+      </c>
+      <c r="B18">
+        <v>22.519747201000001</v>
+      </c>
+      <c r="C18">
+        <v>23.016931944500001</v>
+      </c>
+      <c r="D18">
+        <v>22.691682628999999</v>
+      </c>
+      <c r="E18">
+        <v>22.663869289000001</v>
+      </c>
+      <c r="F18">
+        <v>23.563032184499999</v>
+      </c>
+      <c r="G18">
+        <v>23.576166863099999</v>
+      </c>
+      <c r="H18">
+        <v>22.768766463999999</v>
+      </c>
+      <c r="I18">
+        <v>22.492021857299999</v>
+      </c>
+      <c r="J18">
+        <v>23.459503506699999</v>
+      </c>
+      <c r="K18">
+        <v>22.6967159342</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>22.944843787330001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>50000</v>
+      </c>
+      <c r="B19">
+        <v>22.509238126500001</v>
+      </c>
+      <c r="C19">
+        <v>23.008409930100001</v>
+      </c>
+      <c r="D19">
+        <v>22.683062812199999</v>
+      </c>
+      <c r="E19">
+        <v>22.640481816000001</v>
+      </c>
+      <c r="F19">
+        <v>23.568059510000001</v>
+      </c>
+      <c r="G19">
+        <v>23.4842013835</v>
+      </c>
+      <c r="H19">
+        <v>22.746676750599999</v>
+      </c>
+      <c r="I19">
+        <v>22.497459084599999</v>
+      </c>
+      <c r="J19">
+        <v>23.4943415129</v>
+      </c>
+      <c r="K19">
+        <v>22.696204784300001</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>22.93281357107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>200</v>
+      </c>
+      <c r="B22">
+        <v>13.456470788300001</v>
+      </c>
+      <c r="C22">
+        <v>22.1640838575</v>
+      </c>
+      <c r="D22">
+        <v>20.695855692399999</v>
+      </c>
+      <c r="E22">
+        <v>10.670288236199999</v>
+      </c>
+      <c r="F22">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G22">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="H22">
+        <v>18.444725886299999</v>
+      </c>
+      <c r="I22">
+        <f>AVERAGE(B22:H22)</f>
+        <v>18.953815040385713</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>400</v>
+      </c>
+      <c r="B23">
+        <v>14.1962024812</v>
+      </c>
+      <c r="C23">
+        <v>22.966156476599998</v>
+      </c>
+      <c r="D23">
+        <v>22.483569081300001</v>
+      </c>
+      <c r="E23">
+        <v>16.9965021109</v>
+      </c>
+      <c r="F23">
+        <v>20.8413709039</v>
+      </c>
+      <c r="G23">
+        <v>23.6092630646</v>
+      </c>
+      <c r="H23">
+        <v>11.3986143431</v>
+      </c>
+      <c r="I23">
+        <f t="shared" ref="I23:I39" si="1">AVERAGE(B23:H23)</f>
+        <v>18.92738263737143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>600</v>
+      </c>
+      <c r="B24">
+        <v>15.5930955211</v>
+      </c>
+      <c r="C24">
+        <v>10.649436205200001</v>
+      </c>
+      <c r="D24">
+        <v>19.247360369900001</v>
+      </c>
+      <c r="E24">
+        <v>16.803647980400001</v>
+      </c>
+      <c r="F24">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G24">
+        <v>23.440188042300001</v>
+      </c>
+      <c r="H24">
+        <v>21.963221932300002</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>18.759941494600003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>800</v>
+      </c>
+      <c r="B25">
+        <v>15.0682567783</v>
+      </c>
+      <c r="C25">
+        <v>10.6660322371</v>
+      </c>
+      <c r="D25">
+        <v>16.712383376599998</v>
+      </c>
+      <c r="E25">
+        <v>11.1647521029</v>
+      </c>
+      <c r="F25">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G25">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="H25">
+        <v>19.405523484700002</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>17.180318400228568</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1000</v>
+      </c>
+      <c r="B26">
+        <v>13.561382503500001</v>
+      </c>
+      <c r="C26">
+        <v>23.160194324199999</v>
+      </c>
+      <c r="D26">
+        <v>14.5113579165</v>
+      </c>
+      <c r="E26">
+        <v>18.285196510900001</v>
+      </c>
+      <c r="F26">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G26">
+        <v>23.5943217791</v>
+      </c>
+      <c r="H26">
+        <v>12.5370029543</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>18.467442342785713</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2000</v>
+      </c>
+      <c r="B27">
+        <v>16.951685146700001</v>
+      </c>
+      <c r="C27">
+        <v>23.160154715400001</v>
+      </c>
+      <c r="D27">
+        <v>23.201787022600001</v>
+      </c>
+      <c r="E27">
+        <v>17.805262678599998</v>
+      </c>
+      <c r="F27">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G27">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="H27">
+        <v>22.720990539799999</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>21.583594417871428</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3000</v>
+      </c>
+      <c r="B28">
+        <v>18.8992313189</v>
+      </c>
+      <c r="C28">
+        <v>22.9953405915</v>
+      </c>
+      <c r="D28">
+        <v>11.7235559362</v>
+      </c>
+      <c r="E28">
+        <v>16.4128717006</v>
+      </c>
+      <c r="F28">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G28">
+        <v>23.585855077600002</v>
+      </c>
+      <c r="H28">
+        <v>10.6356889665</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>18.267883428899999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4000</v>
+      </c>
+      <c r="B29">
+        <v>18.348346525099998</v>
+      </c>
+      <c r="C29">
+        <v>23.233031093099999</v>
+      </c>
+      <c r="D29">
+        <v>14.1021016528</v>
+      </c>
+      <c r="E29">
+        <v>16.2214999744</v>
+      </c>
+      <c r="F29">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G29">
+        <v>23.189740438400001</v>
+      </c>
+      <c r="H29">
+        <v>10.6368149362</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>18.47916786157143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5000</v>
+      </c>
+      <c r="B30">
+        <v>18.3759182254</v>
+      </c>
+      <c r="C30">
+        <v>23.161330423300001</v>
+      </c>
+      <c r="D30">
+        <v>14.5269648585</v>
+      </c>
+      <c r="E30">
+        <v>13.5758047134</v>
+      </c>
+      <c r="F30">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G30">
+        <v>23.622296963499998</v>
+      </c>
+      <c r="H30">
+        <v>16.0547284415</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>18.991383433799999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>6000</v>
+      </c>
+      <c r="B31">
+        <v>19.5426545696</v>
+      </c>
+      <c r="C31">
+        <v>23.372765070300002</v>
+      </c>
+      <c r="D31">
+        <v>14.7312470291</v>
+      </c>
+      <c r="E31">
+        <v>22.312814742</v>
+      </c>
+      <c r="F31">
+        <v>21.173767063500001</v>
+      </c>
+      <c r="G31">
+        <v>23.4903590678</v>
+      </c>
+      <c r="H31">
+        <v>15.392385387099999</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>20.002284704200001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>7000</v>
+      </c>
+      <c r="B32">
+        <v>19.447310812800001</v>
+      </c>
+      <c r="C32">
+        <v>23.325893057999998</v>
+      </c>
+      <c r="D32">
+        <v>14.5500060848</v>
+      </c>
+      <c r="E32">
+        <v>19.096585622399999</v>
+      </c>
+      <c r="F32">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G32">
+        <v>22.7977861675</v>
+      </c>
+      <c r="H32">
+        <v>14.1398243536</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>19.568578072871428</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>8000</v>
+      </c>
+      <c r="B33">
+        <v>19.815116947300002</v>
+      </c>
+      <c r="C33">
+        <v>14.818447219499999</v>
+      </c>
+      <c r="D33">
+        <v>14.854156978200001</v>
+      </c>
+      <c r="E33">
+        <v>22.648245795099999</v>
+      </c>
+      <c r="F33">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G33">
+        <v>23.561127503000002</v>
+      </c>
+      <c r="H33">
+        <v>16.454509440199999</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>19.396320613471428</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>9000</v>
+      </c>
+      <c r="B34">
+        <v>20.147942063199999</v>
+      </c>
+      <c r="C34">
+        <v>22.6229098128</v>
+      </c>
+      <c r="D34">
+        <v>15.085827185399999</v>
+      </c>
+      <c r="E34">
+        <v>21.532876762499999</v>
+      </c>
+      <c r="F34">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G34">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="H34">
+        <v>20.948163960700001</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>21.083285800942853</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>10000</v>
+      </c>
+      <c r="B35">
+        <v>21.2898573457</v>
+      </c>
+      <c r="C35">
+        <v>23.5958183931</v>
+      </c>
+      <c r="D35">
+        <v>13.860240795399999</v>
+      </c>
+      <c r="E35">
+        <v>21.361073430800001</v>
+      </c>
+      <c r="F35">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G35">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="H35">
+        <v>15.9724746625</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>20.474963635642858</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>20000</v>
+      </c>
+      <c r="B36">
+        <v>22.675848960500002</v>
+      </c>
+      <c r="C36">
+        <v>23.200114952900002</v>
+      </c>
+      <c r="D36">
+        <v>14.966602529399999</v>
+      </c>
+      <c r="E36">
+        <v>21.451513025899999</v>
+      </c>
+      <c r="F36">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G36">
+        <v>23.5003564722</v>
+      </c>
+      <c r="H36">
+        <v>18.940739054200002</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>21.193973629442858</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>30000</v>
+      </c>
+      <c r="B37">
+        <v>22.656364622600002</v>
+      </c>
+      <c r="C37">
+        <v>23.073251745099999</v>
+      </c>
+      <c r="D37">
+        <v>15.169377609</v>
+      </c>
+      <c r="E37">
+        <v>22.012638771999999</v>
+      </c>
+      <c r="F37">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G37">
+        <v>23.426031825599999</v>
+      </c>
+      <c r="H37">
+        <v>20.698502591899999</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>21.522686796742857</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>40000</v>
+      </c>
+      <c r="B38">
+        <v>22.592000841299999</v>
+      </c>
+      <c r="C38">
+        <v>23.088434778700002</v>
+      </c>
+      <c r="D38">
+        <v>14.9822733977</v>
+      </c>
+      <c r="E38">
+        <v>22.200689585700001</v>
+      </c>
+      <c r="F38">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G38">
+        <v>23.4735201258</v>
+      </c>
+      <c r="H38">
+        <v>19.407167519800002</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>21.338103808571429</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>50000</v>
+      </c>
+      <c r="B39">
+        <v>22.6937107344</v>
+      </c>
+      <c r="C39">
+        <v>23.021278857900001</v>
+      </c>
+      <c r="D39">
+        <v>19.7001261172</v>
+      </c>
+      <c r="E39">
+        <v>22.502527242799999</v>
+      </c>
+      <c r="F39">
+        <v>23.622640410999999</v>
+      </c>
+      <c r="G39">
+        <v>23.464183438100001</v>
+      </c>
+      <c r="H39">
+        <v>22.7608212592</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>22.537898294371434</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>